<commit_message>
added links in bosl velocity bom
</commit_message>
<xml_diff>
--- a/Velocity/Heterodyne/EDA/Velocity BOM.xlsx
+++ b/Velocity/Heterodyne/EDA/Velocity BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\My Documents\Monash\Monash-BoSL\Velocity\Heterodyne\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9CEF3A-2F10-4DF7-84FE-4DBDC82AF136}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD98B3A1-6252-4DD9-A708-75ED0BA25AFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>Part Number</t>
   </si>
@@ -78,9 +78,6 @@
     <t>SMD:CP_Elec_8x10</t>
   </si>
   <si>
-    <t>https://au.mouser.com/ProductDetail/Nichicon/UWT1E331MNL1GS?qs=sGAEpiMZZMsh%252B1woXyUXjxib3yTgZFe2bgHsEDyVhdM%3D</t>
-  </si>
-  <si>
     <t>100 nF</t>
   </si>
   <si>
@@ -178,6 +175,33 @@
   </si>
   <si>
     <t>https://au.element14.com/texas-instruments/ne5532ap/op-amp-dual-low-noise-5532-dip8/dp/1106091</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/panasonic/eeefc1c331p/cap-330-f-16v-radial-smd/dp/9694420?st=330%20micro%20farad%20capacitor</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/multicomp/mc0805b331k500ct/cap-330pf-50v-10-x7r-0805/dp/1759212</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/avx/08055c104kat2a/cap-0-1-f-50v-10-x7r-0805-reel/dp/2280990</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/tdk/c3216x7r1h105k160ab/cap-1-f-50v-10-x7r-1206/dp/1907358</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/vishay/crcw080510k0fkea/res-10k-1-0-125w-0805-thick-film/dp/1469856</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/yageo/rc0805fr-073k3l/res-3k3-1-0-125w-0805-thick-film/dp/9237682</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/vishay/crcw080539k0fkeahp/res-39k-1-0-33w-0805-thick-film/dp/1738980</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/multicomp/mc01w080551k/res-1k-5-0-1w-0805-thick-film/dp/9333711</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/multicomp/mcmr08x3300ftl/res-330r-1-0-125w-0805-ceramic/dp/2073741</t>
   </si>
 </sst>
 </file>
@@ -535,7 +559,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H2" sqref="H2:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,23 +612,26 @@
         <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="3">
         <v>5</v>
       </c>
       <c r="G2" s="5">
-        <v>0.01</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="H2" s="5">
         <f>F2*G2</f>
-        <v>0.05</v>
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -615,25 +642,27 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3">
         <v>3</v>
       </c>
       <c r="G3" s="5">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" ref="H3:H13" si="0">F3*G3</f>
-        <v>0.03</v>
-      </c>
-      <c r="I3" s="2"/>
+        <v>0.09</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -643,26 +672,26 @@
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
       </c>
       <c r="G4" s="5">
-        <v>0.66</v>
+        <v>0.31</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="0"/>
-        <v>0.66</v>
+        <v>0.31</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -670,28 +699,30 @@
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
       </c>
       <c r="G5" s="5">
-        <v>0.01</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-      <c r="I5" s="2"/>
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -701,23 +732,26 @@
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="F6" s="3">
         <v>3</v>
       </c>
       <c r="G6" s="5">
-        <v>0.01</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.309</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -728,23 +762,26 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="5">
-        <v>0.01</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>6.2E-2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -755,23 +792,26 @@
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
       </c>
       <c r="G8" s="5">
-        <v>0.01</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -782,23 +822,26 @@
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="F9" s="3">
         <v>1</v>
       </c>
       <c r="G9" s="5">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -809,38 +852,40 @@
         <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
       </c>
       <c r="G10" s="5">
-        <v>0.01</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="I10" s="2"/>
+        <v>1.2E-2</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
@@ -853,21 +898,21 @@
         <v>3.55</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
@@ -880,21 +925,21 @@
         <v>1.67</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -907,7 +952,7 @@
         <v>2.3199999999999998</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -970,7 +1015,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1" xr:uid="{6E638366-D617-4014-9075-758D2F1B4A30}"/>
+    <hyperlink ref="I5" r:id="rId1" xr:uid="{54E6D206-1583-422A-9C5E-C3783BCD9AE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added enhanced sleeping code for bosl
</commit_message>
<xml_diff>
--- a/Velocity/Heterodyne/EDA/Velocity BOM.xlsx
+++ b/Velocity/Heterodyne/EDA/Velocity BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\My Documents\Monash\Monash-BoSL\Velocity\Heterodyne\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD98B3A1-6252-4DD9-A708-75ED0BA25AFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F225037-D6F6-4119-B100-4887C43D7E3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,9 +183,6 @@
     <t>https://au.element14.com/multicomp/mc0805b331k500ct/cap-330pf-50v-10-x7r-0805/dp/1759212</t>
   </si>
   <si>
-    <t>https://au.element14.com/avx/08055c104kat2a/cap-0-1-f-50v-10-x7r-0805-reel/dp/2280990</t>
-  </si>
-  <si>
     <t>https://au.element14.com/tdk/c3216x7r1h105k160ab/cap-1-f-50v-10-x7r-1206/dp/1907358</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>https://au.element14.com/multicomp/mcmr08x3300ftl/res-330r-1-0-125w-0805-ceramic/dp/2073741</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/avx/08051c104jat2a/cap-0-1-f-100v-5-x7r-0805/dp/2332715</t>
   </si>
 </sst>
 </file>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -721,7 +721,7 @@
         <v>0.53800000000000003</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
         <v>0.309</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -781,7 +781,7 @@
         <v>6.2E-2</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -841,7 +841,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -871,7 +871,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added 4 layer PCB for heterodyne
</commit_message>
<xml_diff>
--- a/Velocity/Heterodyne/EDA/Velocity BOM.xlsx
+++ b/Velocity/Heterodyne/EDA/Velocity BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\My Documents\Monash\Monash-BoSL\Velocity\Heterodyne\EDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User070\scat0009\Documents\Monash-BoSL\Velocity\Heterodyne\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F225037-D6F6-4119-B100-4887C43D7E3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC00955-8E99-45DA-A378-D1CD33CB767E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>Part Number</t>
   </si>
@@ -51,12 +45,6 @@
     <t>QTY per board</t>
   </si>
   <si>
-    <t>Unit Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
     <t xml:space="preserve">Supplier </t>
   </si>
   <si>
@@ -66,18 +54,9 @@
     <t>U2</t>
   </si>
   <si>
-    <t>Any Applicable</t>
-  </si>
-  <si>
-    <t>SMD Capacitor</t>
-  </si>
-  <si>
     <t>0805</t>
   </si>
   <si>
-    <t>SMD:CP_Elec_8x10</t>
-  </si>
-  <si>
     <t>100 nF</t>
   </si>
   <si>
@@ -99,54 +78,21 @@
     <t>C11</t>
   </si>
   <si>
-    <t>330 μF</t>
-  </si>
-  <si>
-    <t>C9,10,12</t>
-  </si>
-  <si>
-    <t>1206</t>
-  </si>
-  <si>
-    <t>C13,14</t>
-  </si>
-  <si>
     <t>1 μF</t>
   </si>
   <si>
     <t>R2</t>
   </si>
   <si>
-    <t>R9</t>
-  </si>
-  <si>
     <t>39 kΩ</t>
   </si>
   <si>
-    <t>R10</t>
-  </si>
-  <si>
     <t>1 kΩ</t>
   </si>
   <si>
-    <t>R11</t>
-  </si>
-  <si>
     <t>330 Ω</t>
   </si>
   <si>
-    <t xml:space="preserve">SO-8 </t>
-  </si>
-  <si>
-    <t>Mixer</t>
-  </si>
-  <si>
-    <t>DIP-8</t>
-  </si>
-  <si>
-    <t>SOT-323, SC-70</t>
-  </si>
-  <si>
     <t>Oscilator</t>
   </si>
   <si>
@@ -156,52 +102,130 @@
     <t>SA612AD</t>
   </si>
   <si>
-    <t>NE5532</t>
-  </si>
-  <si>
     <t>MAX7375AXR105</t>
   </si>
   <si>
-    <t>R6-8</t>
-  </si>
-  <si>
-    <t>C1,2,6-8</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/nxp/sa612ad-01/ic-mixer-osc-double-balanced-8soic/dp/2212081</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/maxim-integrated-products/max7375axr105-t/oscillator-1mhz-5-5v-sc-70-3/dp/2516474?st=MAX7375AXR105</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/texas-instruments/ne5532ap/op-amp-dual-low-noise-5532-dip8/dp/1106091</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/panasonic/eeefc1c331p/cap-330-f-16v-radial-smd/dp/9694420?st=330%20micro%20farad%20capacitor</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/multicomp/mc0805b331k500ct/cap-330pf-50v-10-x7r-0805/dp/1759212</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/tdk/c3216x7r1h105k160ab/cap-1-f-50v-10-x7r-1206/dp/1907358</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/vishay/crcw080510k0fkea/res-10k-1-0-125w-0805-thick-film/dp/1469856</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/yageo/rc0805fr-073k3l/res-3k3-1-0-125w-0805-thick-film/dp/9237682</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/vishay/crcw080539k0fkeahp/res-39k-1-0-33w-0805-thick-film/dp/1738980</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/multicomp/mc01w080551k/res-1k-5-0-1w-0805-thick-film/dp/9333711</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/multicomp/mcmr08x3300ftl/res-330r-1-0-125w-0805-ceramic/dp/2073741</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/avx/08051c104jat2a/cap-0-1-f-100v-5-x7r-0805/dp/2332715</t>
+    <t>1 MHz Ultrasonic Tranducer</t>
+  </si>
+  <si>
+    <t>LS1, LS2</t>
+  </si>
+  <si>
+    <t>C1 - C3</t>
+  </si>
+  <si>
+    <t>SMD Capcitor</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>22 nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4 </t>
+  </si>
+  <si>
+    <t>C5, C6</t>
+  </si>
+  <si>
+    <t>3.3 μF</t>
+  </si>
+  <si>
+    <t>C9, C10, C12</t>
+  </si>
+  <si>
+    <t>C13, C14</t>
+  </si>
+  <si>
+    <t>R1, R3, R6, R10</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>2 kΩ</t>
+  </si>
+  <si>
+    <t>R7, R9</t>
+  </si>
+  <si>
+    <t>R8, R11</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t>RF Mixer</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/nxp-usa-inc/SA612AD-01112/568-1204-5-ND/740395</t>
+  </si>
+  <si>
+    <t>NE5532DR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/NE5532DRG4/296-44326-1-ND/6110600</t>
+  </si>
+  <si>
+    <t>SOT-323/SC-70</t>
+  </si>
+  <si>
+    <t>Unit Price (USD)</t>
+  </si>
+  <si>
+    <t>Total Price (USD)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/maxim-integrated/MAX7375AXR105-T/MAX7375AXR105-TCT-ND/4490142</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/ATMEGA328PB-AU/ATMEGA328PB-AU-ND/5638812</t>
+  </si>
+  <si>
+    <t>ATmega328PB-AU</t>
+  </si>
+  <si>
+    <t>TQFP-32</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>Microcontroler</t>
+  </si>
+  <si>
+    <t>MAX11613</t>
+  </si>
+  <si>
+    <t>MSOP-8</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/maxim-integrated/MAX11613EUA-T/MAX11613EUA-CT-ND/5639977</t>
+  </si>
+  <si>
+    <t>5032-2Pin</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Crystal Oscilator</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/ndk-america-inc/NX5032GA-8.000M-STD-CSU-1/644-1132-1-ND/1788487</t>
+  </si>
+  <si>
+    <t>18 pF</t>
   </si>
 </sst>
 </file>
@@ -264,7 +288,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
@@ -272,8 +296,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -556,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +597,9 @@
     <col min="3" max="3" width="19.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="29.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" style="3" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="3"/>
+    <col min="6" max="6" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="57.5703125" style="3" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" style="3" customWidth="1"/>
     <col min="11" max="16384" width="8.85546875" style="3"/>
@@ -595,427 +625,567 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="3" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F2" s="3">
+        <v>2</v>
+      </c>
+      <c r="G2" s="5">
         <v>5</v>
       </c>
-      <c r="G2" s="5">
-        <v>3.3000000000000002E-2</v>
-      </c>
       <c r="H2" s="5">
-        <f>F2*G2</f>
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>56</v>
+        <f>G2*F2</f>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
+      <c r="B3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3">
         <v>3</v>
       </c>
       <c r="G3" s="5">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="H3" s="5">
-        <f t="shared" ref="H3:H13" si="0">F3*G3</f>
-        <v>0.09</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>49</v>
-      </c>
+        <f t="shared" ref="H3:H31" si="0">G3*F3</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
       </c>
       <c r="G4" s="5">
-        <v>0.31</v>
+        <v>0.1</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="0"/>
-        <v>0.31</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>24</v>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
       </c>
       <c r="G5" s="5">
-        <v>0.26900000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="0"/>
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>50</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3">
         <v>3</v>
       </c>
       <c r="G6" s="5">
-        <v>0.10299999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="0"/>
-        <v>0.309</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>51</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
+      <c r="B7" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="5">
-        <v>6.2E-2</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="0"/>
-        <v>6.2E-2</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>52</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="H8" s="5">
-        <f t="shared" si="0"/>
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="5">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="H9" s="5">
-        <f t="shared" si="0"/>
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
       </c>
       <c r="G10" s="5">
-        <v>1.2E-2</v>
+        <v>0.1</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="0"/>
-        <v>1.2E-2</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>34</v>
+      <c r="B11" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="5">
-        <v>3.55</v>
+        <v>0.1</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="0"/>
-        <v>3.55</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>45</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>36</v>
+      <c r="B12" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>39</v>
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" s="5">
-        <v>1.67</v>
+        <v>0.1</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="0"/>
-        <v>1.67</v>
-      </c>
-      <c r="I12" s="2" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2.29</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="0"/>
+        <v>2.29</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.88</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="5">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="H13" s="5">
-        <f t="shared" si="0"/>
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="7"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="2"/>
+      <c r="G17" s="5">
+        <v>1.56</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="0"/>
+        <v>1.56</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="2"/>
+      <c r="A18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
+        <v>2.71</v>
+      </c>
+      <c r="H18" s="5">
+        <f>F18*G18</f>
+        <v>2.71</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="A19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1.34</v>
+      </c>
+      <c r="H19" s="5">
+        <f>G19*F19</f>
+        <v>1.34</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="B20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C21" s="6"/>
       <c r="E21" s="6"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="H21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="H22" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="D23" s="6"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="H23" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H29" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I5" r:id="rId1" xr:uid="{54E6D206-1583-422A-9C5E-C3783BCD9AE7}"/>
+    <hyperlink ref="I18" r:id="rId1" xr:uid="{7C4D3448-9EDB-4F85-8910-25821B00AB31}"/>
+    <hyperlink ref="I20" r:id="rId2" xr:uid="{8EDD25AB-7C27-4817-91D3-84AA7D00455B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>